<commit_message>
nueva rdp, matrices, p invariantes, etc
</commit_message>
<xml_diff>
--- a/doc/Tabla de eventos y estados.xlsx
+++ b/doc/Tabla de eventos y estados.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Terminal\Desktop\hero\Facultad\Progr Concurrente\TPINTEGRADOR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Terminal\Desktop\hero\Facultad\Progr Concurrente\TPINTEGRADOR\pc-master\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="8820"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>Tablas de Eventos y Estados</t>
   </si>
@@ -123,9 +123,6 @@
     <t>P12</t>
   </si>
   <si>
-    <t>Auto en caja</t>
-  </si>
-  <si>
     <t>T9</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>T13</t>
   </si>
   <si>
-    <t>Auto abona la estadia</t>
-  </si>
-  <si>
     <t>T0</t>
   </si>
   <si>
@@ -268,6 +262,24 @@
   </si>
   <si>
     <t>Cartel apagado</t>
+  </si>
+  <si>
+    <t>T17</t>
+  </si>
+  <si>
+    <t>Auto pago por salida 1</t>
+  </si>
+  <si>
+    <t>Auto pago por salida 2</t>
+  </si>
+  <si>
+    <t>P23</t>
+  </si>
+  <si>
+    <t>Auto en salida 2</t>
+  </si>
+  <si>
+    <t>Auto en salida 1</t>
   </si>
 </sst>
 </file>
@@ -291,8 +303,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -493,9 +505,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -521,6 +530,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -809,7 +821,7 @@
   <dimension ref="B1:F1011"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -880,7 +892,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>14</v>
@@ -908,7 +920,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>21</v>
@@ -936,7 +948,7 @@
         <v>27</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>29</v>
@@ -947,44 +959,44 @@
     </row>
     <row r="11" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>32</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -992,13 +1004,13 @@
         <v>31</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>80</v>
+        <v>38</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1006,167 +1018,177 @@
         <v>33</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>44</v>
+        <v>65</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>68</v>
+        <v>43</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="14" t="s">
+      <c r="C25" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="13"/>
+      <c r="E25" s="12"/>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" s="13"/>
+      <c r="B26" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="12"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B27" s="13"/>
-      <c r="C27" s="2"/>
-      <c r="E27" s="13"/>
+    <row r="27" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="12"/>
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B28" s="13"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B29" s="13"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B30" s="13"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B31" s="13"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="3"/>
@@ -1176,25 +1198,25 @@
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B33" s="13"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B34" s="13"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B35" s="13"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="2:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B36" s="13"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="3"/>
@@ -7033,5 +7055,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>